<commit_message>
Chiran: 894454 user story changes
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C799764
</commit_message>
<xml_diff>
--- a/PPIUK-Phase2/PPIUK-SearchAndBrowse/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Phase2/PPIUK-SearchAndBrowse/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="279">
   <si>
     <t>UserName</t>
   </si>
@@ -844,13 +844,23 @@
   </si>
   <si>
     <t>Global_page111!</t>
+  </si>
+  <si>
+    <t>Search_Browse_User1</t>
+  </si>
+  <si>
+    <t>Search_Browse_User1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,7 +956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -959,6 +969,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1020,7 +1033,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1052,10 +1065,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1087,7 +1099,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1263,24 +1274,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="D106" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1314,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +1335,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1354,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1362,7 +1373,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1404,7 +1415,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1425,7 +1436,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1446,7 +1457,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
         <v>273</v>
       </c>
@@ -1465,7 +1476,7 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1497,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1507,7 +1518,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1528,7 +1539,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1549,7 +1560,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1589,7 +1600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1610,7 +1621,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1629,7 +1640,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -1650,7 +1661,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -1669,7 +1680,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1688,7 +1699,7 @@
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1707,7 +1718,7 @@
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1728,7 +1739,7 @@
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
@@ -1749,7 +1760,7 @@
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
         <v>120</v>
       </c>
@@ -1768,7 +1779,7 @@
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
         <v>56</v>
       </c>
@@ -1787,7 +1798,7 @@
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
         <v>57</v>
       </c>
@@ -1804,7 +1815,7 @@
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -1821,7 +1832,7 @@
       </c>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -1840,7 +1851,7 @@
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
         <v>63</v>
       </c>
@@ -1857,7 +1868,7 @@
       </c>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
@@ -1874,7 +1885,7 @@
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
         <v>271</v>
       </c>
@@ -1893,7 +1904,7 @@
       </c>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">
         <v>74</v>
       </c>
@@ -1912,7 +1923,7 @@
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>80</v>
       </c>
@@ -1931,7 +1942,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>84</v>
       </c>
@@ -1950,7 +1961,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>87</v>
       </c>
@@ -1969,7 +1980,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>88</v>
       </c>
@@ -1988,7 +1999,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>89</v>
       </c>
@@ -2005,7 +2016,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
         <v>90</v>
       </c>
@@ -2024,7 +2035,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
         <v>96</v>
       </c>
@@ -2043,7 +2054,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>99</v>
       </c>
@@ -2066,7 +2077,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
         <v>103</v>
       </c>
@@ -2089,7 +2100,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
         <v>105</v>
       </c>
@@ -2108,7 +2119,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
         <v>109</v>
       </c>
@@ -2129,7 +2140,7 @@
       </c>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
         <v>110</v>
       </c>
@@ -2150,7 +2161,7 @@
       </c>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -2173,7 +2184,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="7" t="s">
         <v>116</v>
       </c>
@@ -2192,7 +2203,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="7" t="s">
         <v>117</v>
       </c>
@@ -2211,7 +2222,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>123</v>
       </c>
@@ -2232,7 +2243,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
         <v>127</v>
       </c>
@@ -2253,7 +2264,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
         <v>132</v>
       </c>
@@ -2274,7 +2285,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
         <v>137</v>
       </c>
@@ -2293,7 +2304,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="5" t="s">
         <v>139</v>
       </c>
@@ -2312,7 +2323,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
         <v>141</v>
       </c>
@@ -2331,7 +2342,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>144</v>
       </c>
@@ -2348,7 +2359,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -2365,7 +2376,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>146</v>
       </c>
@@ -2382,7 +2393,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>147</v>
       </c>
@@ -2399,7 +2410,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>148</v>
       </c>
@@ -2416,7 +2427,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -2433,7 +2444,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>150</v>
       </c>
@@ -2450,7 +2461,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>151</v>
       </c>
@@ -2467,7 +2478,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>152</v>
       </c>
@@ -2484,7 +2495,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>153</v>
       </c>
@@ -2501,7 +2512,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>154</v>
       </c>
@@ -2518,7 +2529,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -2535,7 +2546,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>156</v>
       </c>
@@ -2552,7 +2563,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>157</v>
       </c>
@@ -2569,7 +2580,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>158</v>
       </c>
@@ -2586,7 +2597,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>159</v>
       </c>
@@ -2603,7 +2614,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>160</v>
       </c>
@@ -2620,7 +2631,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>161</v>
       </c>
@@ -2637,7 +2648,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -2654,7 +2665,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -2671,7 +2682,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>164</v>
       </c>
@@ -2688,7 +2699,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>165</v>
       </c>
@@ -2705,7 +2716,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>166</v>
       </c>
@@ -2722,7 +2733,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -2739,7 +2750,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>168</v>
       </c>
@@ -2756,7 +2767,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -2773,7 +2784,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -2790,7 +2801,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -2807,7 +2818,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7">
       <c r="A82" s="11" t="s">
         <v>205</v>
       </c>
@@ -2824,7 +2835,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="A83" s="11" t="s">
         <v>207</v>
       </c>
@@ -2841,7 +2852,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" s="11" t="s">
         <v>209</v>
       </c>
@@ -2858,7 +2869,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" s="11" t="s">
         <v>211</v>
       </c>
@@ -2875,7 +2886,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" s="11" t="s">
         <v>213</v>
       </c>
@@ -2892,7 +2903,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="A87" s="11" t="s">
         <v>215</v>
       </c>
@@ -2909,7 +2920,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7">
       <c r="A88" s="11" t="s">
         <v>217</v>
       </c>
@@ -2926,7 +2937,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" s="11" t="s">
         <v>219</v>
       </c>
@@ -2943,7 +2954,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="A90" s="11" t="s">
         <v>221</v>
       </c>
@@ -2960,7 +2971,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7">
       <c r="A91" s="11" t="s">
         <v>223</v>
       </c>
@@ -2977,7 +2988,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="A92" s="11" t="s">
         <v>225</v>
       </c>
@@ -2994,7 +3005,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="A93" s="11" t="s">
         <v>227</v>
       </c>
@@ -3011,7 +3022,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="A94" s="11" t="s">
         <v>229</v>
       </c>
@@ -3028,7 +3039,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="A95" s="11" t="s">
         <v>231</v>
       </c>
@@ -3045,7 +3056,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7">
       <c r="A96" s="11" t="s">
         <v>233</v>
       </c>
@@ -3062,7 +3073,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7">
       <c r="A97" s="11" t="s">
         <v>235</v>
       </c>
@@ -3079,7 +3090,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" s="11" t="s">
         <v>237</v>
       </c>
@@ -3096,7 +3107,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="A99" s="11" t="s">
         <v>239</v>
       </c>
@@ -3113,7 +3124,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" s="11" t="s">
         <v>241</v>
       </c>
@@ -3130,7 +3141,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" s="11" t="s">
         <v>243</v>
       </c>
@@ -3147,7 +3158,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" s="11" t="s">
         <v>245</v>
       </c>
@@ -3164,7 +3175,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="11" t="s">
         <v>247</v>
       </c>
@@ -3181,7 +3192,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="11" t="s">
         <v>249</v>
       </c>
@@ -3198,7 +3209,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7">
       <c r="A105" s="11" t="s">
         <v>251</v>
       </c>
@@ -3215,7 +3226,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7">
       <c r="A106" s="11" t="s">
         <v>253</v>
       </c>
@@ -3232,7 +3243,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7">
       <c r="A107" s="11" t="s">
         <v>255</v>
       </c>
@@ -3249,7 +3260,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7">
       <c r="A108" s="11" t="s">
         <v>257</v>
       </c>
@@ -3266,7 +3277,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7">
       <c r="A109" s="11" t="s">
         <v>259</v>
       </c>
@@ -3283,7 +3294,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7">
       <c r="A110" s="11" t="s">
         <v>261</v>
       </c>
@@ -3300,7 +3311,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7">
       <c r="A111" s="11" t="s">
         <v>263</v>
       </c>
@@ -3317,7 +3328,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7">
       <c r="A112" s="11" t="s">
         <v>265</v>
       </c>
@@ -3334,7 +3345,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7">
       <c r="A113" s="11" t="s">
         <v>267</v>
       </c>
@@ -3351,7 +3362,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7">
       <c r="A114" s="11" t="s">
         <v>269</v>
       </c>
@@ -3366,6 +3377,23 @@
       </c>
       <c r="G114" s="10" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>276</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3446,27 +3474,28 @@
     <hyperlink ref="G111" r:id="rId74"/>
     <hyperlink ref="G114" r:id="rId75"/>
     <hyperlink ref="G112" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G115" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3474,7 +3503,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>202</v>
       </c>
@@ -3482,7 +3511,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -3496,12 +3525,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>